<commit_message>
did some changes to KB,GQ,RQ ,add some new images
</commit_message>
<xml_diff>
--- a/src/KB.xlsx
+++ b/src/KB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HASHINI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nutricarenew\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F540F4-173B-4E11-A3A4-51EC6BEF3E25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{94FBC6BA-BDB8-4B58-905F-08AF823A1E1B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1593,8 +1592,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1614,16 +1613,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1631,21 +1650,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent6" xfId="1" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1957,11 +1996,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAC51A0-A3E9-4852-B2DC-59D7B4A9F9B9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.5"/>
@@ -1978,11 +2017,11 @@
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="51.6" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="51.6" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -2007,1457 +2046,1457 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="335.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" ht="335.4" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" ht="373.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="373.8" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" ht="409.2" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="409.2" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="297" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="297" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="D9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="275.39999999999998" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="H11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="275.39999999999998" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="D12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="362.4" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H18" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G19" s="3" t="s">
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="362.4" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="D20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I20" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="3" t="s">
+      <c r="D21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="3" t="s">
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="3" t="s">
+      <c r="D23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I23" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="3" t="s">
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="3" t="s">
+      <c r="H24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G25" s="3" t="s">
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="3" t="s">
+      <c r="H25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="D26" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="3" t="s">
+      <c r="H26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="3" t="s">
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="3" t="s">
+      <c r="H27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G28" s="3" t="s">
+      <c r="D28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G29" s="3" t="s">
+      <c r="E29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G30" s="3" t="s">
+      <c r="E30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G31" s="3" t="s">
+      <c r="E31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3" t="s">
+      <c r="E32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="D33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G33" s="3" t="s">
+      <c r="F33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G34" s="3" t="s">
+      <c r="F34" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="D35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G35" s="3" t="s">
+      <c r="F35" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="D36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G36" s="3" t="s">
+      <c r="F36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H36" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="3" t="s">
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A40" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="3" t="s">
+      <c r="D40" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G41" s="3" t="s">
+      <c r="D41" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A42" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G42" s="3" t="s">
+      <c r="D42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="3" t="s">
+      <c r="D43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G44" s="3" t="s">
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="H44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H45" s="3" t="s">
+      <c r="H45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="409.6" x14ac:dyDescent="0.5">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="D46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H46" s="3" t="s">
+      <c r="H46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I46" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A47" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H47" s="3" t="s">
+      <c r="H47" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I47" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="405.6" x14ac:dyDescent="0.5">
       <c r="A48" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="D48" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H48" s="3" t="s">
+      <c r="H48" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+      <c r="I48" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A49" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G49" s="3" t="s">
+      <c r="D49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I49" s="3" t="s">
+      <c r="H49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:9" ht="376.8" x14ac:dyDescent="0.5">
       <c r="A50" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="3" t="s">
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H50" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I50" s="3" t="s">
+      <c r="H50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="1" customFormat="1" ht="409.6" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:9" ht="391.2" x14ac:dyDescent="0.5">
       <c r="A51" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="D51" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I51" s="3" t="s">
+      <c r="H51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.5">
       <c r="C52" s="1" t="s">
         <v>91</v>
       </c>
@@ -3483,5 +3522,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>